<commit_message>
Bug fixes after MEX updates
</commit_message>
<xml_diff>
--- a/Curves/sedan_DecelCurve.xlsx
+++ b/Curves/sedan_DecelCurve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\codex\z\VDSS---Vehicle-Dynamics-Safety-Simulator\Curves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA390764-CA71-49ED-A7FC-D451C1E2927F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBE936B-2E6D-47E9-9C51-2025D02ABA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="92955" yWindow="990" windowWidth="21600" windowHeight="11423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="86303" yWindow="-98" windowWidth="28995" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -196,102 +196,81 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$32</c:f>
+              <c:f>Sheet1!$B$2:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>-0.8</c:v>
+                  <c:v>-2.4230514575044602</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.8</c:v>
+                  <c:v>-2.1869262666181899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.9524242114449399</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.71959152131576</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.48847749822579</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.2591348467896999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.8</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.8</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-1.03162005421553</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-1.2591348467896999</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>-1.48847749822579</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-1.71959152131576</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-1.9524242114449399</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>-2.1869262666181899</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>-2.4230514575044602</c:v>
+                  <c:v>-1.03162005421553</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1364,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-0.8</v>
+        <v>-2.4230514575044602</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -1372,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.8</v>
+        <v>-2.1869262666181899</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -1380,7 +1359,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.8</v>
+        <v>-1.9524242114449399</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -1388,7 +1367,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-0.8</v>
+        <v>-1.71959152131576</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -1396,7 +1375,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-0.8</v>
+        <v>-1.48847749822579</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -1404,7 +1383,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.8</v>
+        <v>-1.2591348467896999</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -1412,7 +1391,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
@@ -1420,7 +1399,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
@@ -1428,7 +1407,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
@@ -1436,7 +1415,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
@@ -1444,7 +1423,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
@@ -1452,7 +1431,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
@@ -1460,7 +1439,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
@@ -1468,7 +1447,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
@@ -1476,7 +1455,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
@@ -1484,7 +1463,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
@@ -1492,7 +1471,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
@@ -1500,7 +1479,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
@@ -1508,7 +1487,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
@@ -1516,7 +1495,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
@@ -1524,7 +1503,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
@@ -1532,7 +1511,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
@@ -1540,7 +1519,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
@@ -1548,7 +1527,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>-0.8</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
@@ -1564,7 +1543,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>-1.2591348467896999</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
@@ -1572,7 +1551,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>-1.48847749822579</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
@@ -1580,7 +1559,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>-1.71959152131576</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
@@ -1588,7 +1567,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>-1.9524242114449399</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
@@ -1596,7 +1575,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>-2.1869262666181899</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
@@ -1604,7 +1583,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>-2.4230514575044602</v>
+        <v>-1.03162005421553</v>
       </c>
     </row>
   </sheetData>

</xml_diff>